<commit_message>
Tuesday Office 1:36 PM 6/21/22
</commit_message>
<xml_diff>
--- a/details/Chicagoland Telecom Pricing.xlsx
+++ b/details/Chicagoland Telecom Pricing.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nic Wehrwein\Desktop\Ops_Nic_1\Notes\Transition\Training\Price Guides\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\internet_tv_cal\details\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192701ED-B400-46AB-925D-91595158DAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{3727727B-05F2-4165-8EC3-942BF6475957}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Comcast" sheetId="1" r:id="rId1"/>
@@ -261,7 +260,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -765,7 +764,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A82BBBD-0054-4473-8ACE-06C0B10F11D1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -1077,14 +1076,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB943C1-BEFC-43AF-A2E6-3388E28196AE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:B27"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,14 +1347,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15EB77AD-D28A-4068-833F-A145C2F2AE50}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,7 +1644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795F9376-C52B-4204-8066-46997D628037}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
@@ -1712,13 +1711,13 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53DE4900-4973-4F62-8C8F-17134BF127E9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>

</xml_diff>